<commit_message>
added velocity profiles to supplemental file
</commit_message>
<xml_diff>
--- a/static/documents/Supplemental_info.xlsx
+++ b/static/documents/Supplemental_info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\blucci\Desktop\piv\static\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37A760B-E4DA-41FC-9EE8-E0FC12076858}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E4EFA2-F930-41E8-BDEB-D6234B112328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestChart" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Array Descriptions" sheetId="7" r:id="rId3"/>
     <sheet name="SmoothEndwallLimits" sheetId="12" r:id="rId4"/>
     <sheet name="GeometryParameters" sheetId="13" r:id="rId5"/>
+    <sheet name="InletVelocityProfile" sheetId="14" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="diary." localSheetId="2">'Array Descriptions'!$A$1:$C$37</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="515">
   <si>
     <t>Q25_smooth_small_sc655</t>
   </si>
@@ -2204,12 +2205,36 @@
   <si>
     <t>Limits for Plotting</t>
   </si>
+  <si>
+    <t>flow rate 0.28</t>
+  </si>
+  <si>
+    <t>flow rate 0.38</t>
+  </si>
+  <si>
+    <t>Uz(m/s)</t>
+  </si>
+  <si>
+    <t>r/L</t>
+  </si>
+  <si>
+    <t>L=45.7mm</t>
+  </si>
+  <si>
+    <t>kinematic viscosity at the experimental temperature is 1.1X10-6 m2/s.</t>
+  </si>
+  <si>
+    <t>The working fluid is a sodium iodide solution.</t>
+  </si>
+  <si>
+    <t>The specific gravity of the solution is 1.8 and</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2361,6 +2386,28 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="32"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3251,7 +3298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -3438,19 +3485,46 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3462,46 +3536,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3537,48 +3575,62 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7352,7 +7404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="D1:P70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
@@ -7384,51 +7436,51 @@
       <c r="D4" s="10" t="s">
         <v>396</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="121" t="s">
         <v>397</v>
       </c>
-      <c r="F4" s="77"/>
+      <c r="F4" s="122"/>
       <c r="G4" s="11" t="s">
         <v>398</v>
       </c>
-      <c r="H4" s="76" t="s">
+      <c r="H4" s="121" t="s">
         <v>399</v>
       </c>
-      <c r="I4" s="77"/>
+      <c r="I4" s="122"/>
       <c r="J4" s="12" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="5" spans="4:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="78" t="s">
+      <c r="D5" s="109" t="s">
         <v>401</v>
       </c>
-      <c r="E5" s="80" t="s">
+      <c r="E5" s="82" t="s">
         <v>402</v>
       </c>
-      <c r="F5" s="81"/>
+      <c r="F5" s="90"/>
       <c r="G5" s="61">
         <v>0.25</v>
       </c>
-      <c r="H5" s="84" t="s">
+      <c r="H5" s="111" t="s">
         <v>403</v>
       </c>
-      <c r="I5" s="85"/>
+      <c r="I5" s="112"/>
       <c r="J5" s="13">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D6" s="79"/>
-      <c r="E6" s="82"/>
-      <c r="F6" s="83"/>
+      <c r="D6" s="110"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="92"/>
       <c r="G6" s="62">
         <v>0.35</v>
       </c>
-      <c r="H6" s="86" t="s">
+      <c r="H6" s="113" t="s">
         <v>403</v>
       </c>
-      <c r="I6" s="87"/>
+      <c r="I6" s="114"/>
       <c r="J6" s="14">
         <v>6</v>
       </c>
@@ -7443,35 +7495,35 @@
       <c r="J7" s="15"/>
     </row>
     <row r="8" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D8" s="78" t="s">
+      <c r="D8" s="109" t="s">
         <v>404</v>
       </c>
-      <c r="E8" s="80" t="s">
+      <c r="E8" s="82" t="s">
         <v>402</v>
       </c>
-      <c r="F8" s="81"/>
+      <c r="F8" s="90"/>
       <c r="G8" s="61">
         <v>0.25</v>
       </c>
-      <c r="H8" s="84" t="s">
+      <c r="H8" s="111" t="s">
         <v>403</v>
       </c>
-      <c r="I8" s="85"/>
+      <c r="I8" s="112"/>
       <c r="J8" s="13">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="4:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="79"/>
-      <c r="E9" s="82"/>
-      <c r="F9" s="83"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="91"/>
+      <c r="F9" s="92"/>
       <c r="G9" s="62">
         <v>0.35</v>
       </c>
-      <c r="H9" s="86" t="s">
+      <c r="H9" s="113" t="s">
         <v>403</v>
       </c>
-      <c r="I9" s="87"/>
+      <c r="I9" s="114"/>
       <c r="J9" s="14">
         <v>14</v>
       </c>
@@ -7486,10 +7538,10 @@
       <c r="J10" s="19"/>
     </row>
     <row r="11" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="88" t="s">
+      <c r="D11" s="115" t="s">
         <v>405</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="76" t="s">
         <v>402</v>
       </c>
       <c r="F11" s="65" t="s">
@@ -7510,8 +7562,8 @@
       <c r="K11" s="23"/>
     </row>
     <row r="12" spans="4:16" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="89"/>
-      <c r="E12" s="90"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="77"/>
       <c r="F12" s="24"/>
       <c r="G12" s="20"/>
       <c r="H12" s="20"/>
@@ -7519,9 +7571,9 @@
       <c r="J12" s="25"/>
     </row>
     <row r="13" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D13" s="89"/>
-      <c r="E13" s="89"/>
-      <c r="F13" s="92" t="s">
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
+      <c r="F13" s="76" t="s">
         <v>408</v>
       </c>
       <c r="G13" s="26">
@@ -7538,64 +7590,64 @@
       </c>
     </row>
     <row r="14" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="94">
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="118">
         <v>0.35</v>
       </c>
       <c r="H14" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="I14" s="95" t="s">
+      <c r="I14" s="119" t="s">
         <v>403</v>
       </c>
-      <c r="J14" s="98">
+      <c r="J14" s="95">
         <v>14</v>
       </c>
     </row>
     <row r="15" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D15" s="89"/>
-      <c r="E15" s="89"/>
-      <c r="F15" s="90"/>
-      <c r="G15" s="94"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="118"/>
       <c r="H15" s="63" t="s">
         <v>409</v>
       </c>
-      <c r="I15" s="96"/>
-      <c r="J15" s="99"/>
+      <c r="I15" s="120"/>
+      <c r="J15" s="96"/>
     </row>
     <row r="16" spans="4:16" x14ac:dyDescent="0.3">
-      <c r="D16" s="89"/>
-      <c r="E16" s="89"/>
-      <c r="F16" s="90"/>
-      <c r="G16" s="100">
+      <c r="D16" s="116"/>
+      <c r="E16" s="116"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="97">
         <v>0.38</v>
       </c>
       <c r="H16" s="57" t="s">
         <v>407</v>
       </c>
-      <c r="I16" s="102" t="s">
+      <c r="I16" s="99" t="s">
         <v>403</v>
       </c>
-      <c r="J16" s="104">
+      <c r="J16" s="101">
         <v>14</v>
       </c>
     </row>
     <row r="17" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="89"/>
-      <c r="E17" s="89"/>
-      <c r="F17" s="93"/>
-      <c r="G17" s="101"/>
+      <c r="D17" s="116"/>
+      <c r="E17" s="116"/>
+      <c r="F17" s="79"/>
+      <c r="G17" s="98"/>
       <c r="H17" s="58" t="s">
         <v>409</v>
       </c>
-      <c r="I17" s="103"/>
-      <c r="J17" s="105"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="102"/>
     </row>
     <row r="18" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="89"/>
-      <c r="E18" s="90"/>
+      <c r="D18" s="116"/>
+      <c r="E18" s="77"/>
       <c r="F18" s="30"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
@@ -7603,8 +7655,8 @@
       <c r="J18" s="32"/>
     </row>
     <row r="19" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="89"/>
-      <c r="E19" s="93"/>
+      <c r="D19" s="116"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="33" t="s">
         <v>410</v>
       </c>
@@ -7622,7 +7674,7 @@
       </c>
     </row>
     <row r="20" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="90"/>
+      <c r="D20" s="77"/>
       <c r="E20" s="29"/>
       <c r="F20" s="29"/>
       <c r="G20" s="29"/>
@@ -7631,57 +7683,57 @@
       <c r="J20" s="29"/>
     </row>
     <row r="21" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D21" s="89"/>
-      <c r="E21" s="92" t="s">
+      <c r="D21" s="116"/>
+      <c r="E21" s="76" t="s">
         <v>411</v>
       </c>
-      <c r="F21" s="106" t="s">
+      <c r="F21" s="103" t="s">
         <v>412</v>
       </c>
       <c r="G21" s="26">
         <v>0.25</v>
       </c>
-      <c r="H21" s="97" t="s">
+      <c r="H21" s="106" t="s">
         <v>413</v>
       </c>
-      <c r="I21" s="97"/>
+      <c r="I21" s="106"/>
       <c r="J21" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D22" s="89"/>
-      <c r="E22" s="90"/>
-      <c r="F22" s="107"/>
+      <c r="D22" s="116"/>
+      <c r="E22" s="77"/>
+      <c r="F22" s="104"/>
       <c r="G22" s="56">
         <v>0.35</v>
       </c>
-      <c r="H22" s="109" t="s">
+      <c r="H22" s="107" t="s">
         <v>413</v>
       </c>
-      <c r="I22" s="109"/>
+      <c r="I22" s="107"/>
       <c r="J22" s="37">
         <v>14</v>
       </c>
     </row>
     <row r="23" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="89"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="108"/>
+      <c r="D23" s="116"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="105"/>
       <c r="G23" s="69">
         <v>0.38</v>
       </c>
-      <c r="H23" s="110" t="s">
+      <c r="H23" s="108" t="s">
         <v>413</v>
       </c>
-      <c r="I23" s="110"/>
+      <c r="I23" s="108"/>
       <c r="J23" s="38">
         <v>14</v>
       </c>
     </row>
     <row r="24" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="89"/>
-      <c r="E24" s="90"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="77"/>
       <c r="F24" s="39"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
@@ -7689,33 +7741,33 @@
       <c r="J24" s="40"/>
     </row>
     <row r="25" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="89"/>
-      <c r="E25" s="90"/>
-      <c r="F25" s="106" t="s">
+      <c r="D25" s="116"/>
+      <c r="E25" s="77"/>
+      <c r="F25" s="103" t="s">
         <v>414</v>
       </c>
       <c r="G25" s="26">
         <v>0.35</v>
       </c>
-      <c r="H25" s="97" t="s">
+      <c r="H25" s="106" t="s">
         <v>413</v>
       </c>
-      <c r="I25" s="97"/>
+      <c r="I25" s="106"/>
       <c r="J25" s="28">
         <v>14</v>
       </c>
     </row>
     <row r="26" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="91"/>
-      <c r="E26" s="93"/>
-      <c r="F26" s="108"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="79"/>
+      <c r="F26" s="105"/>
       <c r="G26" s="69">
         <v>0.38</v>
       </c>
-      <c r="H26" s="110" t="s">
+      <c r="H26" s="108" t="s">
         <v>413</v>
       </c>
-      <c r="I26" s="110"/>
+      <c r="I26" s="108"/>
       <c r="J26" s="38">
         <v>14</v>
       </c>
@@ -7730,55 +7782,55 @@
       <c r="J27" s="16"/>
     </row>
     <row r="28" spans="4:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="92" t="s">
+      <c r="D28" s="76" t="s">
         <v>415</v>
       </c>
-      <c r="E28" s="92" t="s">
+      <c r="E28" s="76" t="s">
         <v>416</v>
       </c>
-      <c r="F28" s="112" t="s">
+      <c r="F28" s="80" t="s">
         <v>417</v>
       </c>
       <c r="G28" s="60">
         <v>0.25</v>
       </c>
-      <c r="H28" s="80" t="s">
+      <c r="H28" s="82" t="s">
         <v>413</v>
       </c>
-      <c r="I28" s="114"/>
+      <c r="I28" s="83"/>
       <c r="J28" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="29" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D29" s="90"/>
-      <c r="E29" s="90"/>
-      <c r="F29" s="111"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="78"/>
       <c r="G29" s="42">
         <v>0.35</v>
       </c>
-      <c r="H29" s="115"/>
-      <c r="I29" s="116"/>
+      <c r="H29" s="84"/>
+      <c r="I29" s="85"/>
       <c r="J29" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="30" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="113"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="81"/>
       <c r="G30" s="59">
         <v>0.38</v>
       </c>
-      <c r="H30" s="117"/>
-      <c r="I30" s="118"/>
+      <c r="H30" s="86"/>
+      <c r="I30" s="87"/>
       <c r="J30" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="90"/>
-      <c r="E31" s="111"/>
+      <c r="D31" s="77"/>
+      <c r="E31" s="78"/>
       <c r="F31" s="45"/>
       <c r="G31" s="46"/>
       <c r="H31" s="46"/>
@@ -7786,50 +7838,50 @@
       <c r="J31" s="47"/>
     </row>
     <row r="32" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="112" t="s">
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="80" t="s">
         <v>414</v>
       </c>
       <c r="G32" s="60">
         <v>0.25</v>
       </c>
-      <c r="H32" s="80" t="s">
+      <c r="H32" s="82" t="s">
         <v>418</v>
       </c>
-      <c r="I32" s="114"/>
+      <c r="I32" s="83"/>
       <c r="J32" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="33" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D33" s="90"/>
-      <c r="E33" s="90"/>
-      <c r="F33" s="111"/>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="78"/>
       <c r="G33" s="42">
         <v>0.35</v>
       </c>
-      <c r="H33" s="115"/>
-      <c r="I33" s="116"/>
+      <c r="H33" s="84"/>
+      <c r="I33" s="85"/>
       <c r="J33" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="34" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="90"/>
-      <c r="E34" s="93"/>
-      <c r="F34" s="113"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="79"/>
+      <c r="F34" s="81"/>
       <c r="G34" s="59">
         <v>0.38</v>
       </c>
-      <c r="H34" s="117"/>
-      <c r="I34" s="118"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="87"/>
       <c r="J34" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="35" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D35" s="111"/>
+      <c r="D35" s="78"/>
       <c r="E35" s="45"/>
       <c r="F35" s="45"/>
       <c r="G35" s="46"/>
@@ -7838,53 +7890,53 @@
       <c r="J35" s="47"/>
     </row>
     <row r="36" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D36" s="90"/>
-      <c r="E36" s="92" t="s">
+      <c r="D36" s="77"/>
+      <c r="E36" s="76" t="s">
         <v>419</v>
       </c>
-      <c r="F36" s="112" t="s">
+      <c r="F36" s="80" t="s">
         <v>420</v>
       </c>
       <c r="G36" s="60">
         <v>0.25</v>
       </c>
-      <c r="H36" s="80" t="s">
+      <c r="H36" s="82" t="s">
         <v>403</v>
       </c>
-      <c r="I36" s="114"/>
+      <c r="I36" s="83"/>
       <c r="J36" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="37" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D37" s="90"/>
-      <c r="E37" s="90"/>
-      <c r="F37" s="111"/>
+      <c r="D37" s="77"/>
+      <c r="E37" s="77"/>
+      <c r="F37" s="78"/>
       <c r="G37" s="42">
         <v>0.35</v>
       </c>
-      <c r="H37" s="115"/>
-      <c r="I37" s="116"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="85"/>
       <c r="J37" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="38" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="113"/>
+      <c r="D38" s="77"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="81"/>
       <c r="G38" s="59">
         <v>0.38</v>
       </c>
-      <c r="H38" s="117"/>
-      <c r="I38" s="118"/>
+      <c r="H38" s="86"/>
+      <c r="I38" s="87"/>
       <c r="J38" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="39" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="90"/>
-      <c r="E39" s="111"/>
+      <c r="D39" s="77"/>
+      <c r="E39" s="78"/>
       <c r="F39" s="45"/>
       <c r="G39" s="46"/>
       <c r="H39" s="46"/>
@@ -7892,51 +7944,51 @@
       <c r="J39" s="47"/>
     </row>
     <row r="40" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D40" s="90"/>
-      <c r="E40" s="90"/>
-      <c r="F40" s="112" t="s">
+      <c r="D40" s="77"/>
+      <c r="E40" s="77"/>
+      <c r="F40" s="80" t="s">
         <v>421</v>
       </c>
       <c r="G40" s="60">
         <v>0.25</v>
       </c>
-      <c r="H40" s="80" t="s">
+      <c r="H40" s="82" t="s">
         <v>403</v>
       </c>
-      <c r="I40" s="114"/>
+      <c r="I40" s="83"/>
       <c r="J40" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="41" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="D41" s="90"/>
-      <c r="E41" s="90"/>
-      <c r="F41" s="111"/>
+      <c r="D41" s="77"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="78"/>
       <c r="G41" s="42">
         <v>0.35</v>
       </c>
-      <c r="H41" s="115"/>
-      <c r="I41" s="116"/>
+      <c r="H41" s="84"/>
+      <c r="I41" s="85"/>
       <c r="J41" s="43">
         <v>14</v>
       </c>
       <c r="O41" s="48"/>
     </row>
     <row r="42" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="90"/>
-      <c r="E42" s="93"/>
-      <c r="F42" s="113"/>
+      <c r="D42" s="77"/>
+      <c r="E42" s="79"/>
+      <c r="F42" s="81"/>
       <c r="G42" s="59">
         <v>0.38</v>
       </c>
-      <c r="H42" s="117"/>
-      <c r="I42" s="118"/>
+      <c r="H42" s="86"/>
+      <c r="I42" s="87"/>
       <c r="J42" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="43" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="111"/>
+      <c r="D43" s="78"/>
       <c r="E43" s="45"/>
       <c r="F43" s="45"/>
       <c r="G43" s="46"/>
@@ -7945,33 +7997,33 @@
       <c r="J43" s="47"/>
     </row>
     <row r="44" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D44" s="90"/>
-      <c r="E44" s="112" t="s">
+      <c r="D44" s="77"/>
+      <c r="E44" s="80" t="s">
         <v>422</v>
       </c>
-      <c r="F44" s="119" t="s">
+      <c r="F44" s="88" t="s">
         <v>423</v>
       </c>
       <c r="G44" s="60">
         <v>0.25</v>
       </c>
-      <c r="H44" s="80" t="s">
+      <c r="H44" s="82" t="s">
         <v>424</v>
       </c>
-      <c r="I44" s="81"/>
+      <c r="I44" s="90"/>
       <c r="J44" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="4:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D45" s="93"/>
-      <c r="E45" s="113"/>
-      <c r="F45" s="120"/>
+      <c r="D45" s="79"/>
+      <c r="E45" s="81"/>
+      <c r="F45" s="89"/>
       <c r="G45" s="59">
         <v>0.38</v>
       </c>
-      <c r="H45" s="82"/>
-      <c r="I45" s="83"/>
+      <c r="H45" s="91"/>
+      <c r="I45" s="92"/>
       <c r="J45" s="44">
         <v>1</v>
       </c>
@@ -7986,55 +8038,55 @@
       <c r="J46" s="51"/>
     </row>
     <row r="47" spans="4:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D47" s="92" t="s">
+      <c r="D47" s="76" t="s">
         <v>425</v>
       </c>
-      <c r="E47" s="92" t="s">
+      <c r="E47" s="76" t="s">
         <v>416</v>
       </c>
-      <c r="F47" s="112" t="s">
+      <c r="F47" s="80" t="s">
         <v>417</v>
       </c>
       <c r="G47" s="60">
         <v>0.25</v>
       </c>
-      <c r="H47" s="80" t="s">
+      <c r="H47" s="82" t="s">
         <v>418</v>
       </c>
-      <c r="I47" s="114"/>
+      <c r="I47" s="83"/>
       <c r="J47" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="48" spans="4:15" x14ac:dyDescent="0.3">
-      <c r="D48" s="90"/>
-      <c r="E48" s="90"/>
-      <c r="F48" s="111"/>
+      <c r="D48" s="77"/>
+      <c r="E48" s="77"/>
+      <c r="F48" s="78"/>
       <c r="G48" s="42">
         <v>0.35</v>
       </c>
-      <c r="H48" s="115"/>
-      <c r="I48" s="116"/>
+      <c r="H48" s="84"/>
+      <c r="I48" s="85"/>
       <c r="J48" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="49" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="90"/>
-      <c r="E49" s="90"/>
-      <c r="F49" s="113"/>
+      <c r="D49" s="77"/>
+      <c r="E49" s="77"/>
+      <c r="F49" s="81"/>
       <c r="G49" s="59">
         <v>0.38</v>
       </c>
-      <c r="H49" s="117"/>
-      <c r="I49" s="118"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="87"/>
       <c r="J49" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="50" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="90"/>
-      <c r="E50" s="111"/>
+      <c r="D50" s="77"/>
+      <c r="E50" s="78"/>
       <c r="F50" s="45"/>
       <c r="G50" s="46"/>
       <c r="H50" s="46"/>
@@ -8042,50 +8094,50 @@
       <c r="J50" s="47"/>
     </row>
     <row r="51" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D51" s="90"/>
-      <c r="E51" s="90"/>
-      <c r="F51" s="112" t="s">
+      <c r="D51" s="77"/>
+      <c r="E51" s="77"/>
+      <c r="F51" s="80" t="s">
         <v>414</v>
       </c>
       <c r="G51" s="60">
         <v>0.25</v>
       </c>
-      <c r="H51" s="80" t="s">
+      <c r="H51" s="82" t="s">
         <v>418</v>
       </c>
-      <c r="I51" s="114"/>
+      <c r="I51" s="83"/>
       <c r="J51" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="52" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D52" s="90"/>
-      <c r="E52" s="90"/>
-      <c r="F52" s="111"/>
+      <c r="D52" s="77"/>
+      <c r="E52" s="77"/>
+      <c r="F52" s="78"/>
       <c r="G52" s="42">
         <v>0.35</v>
       </c>
-      <c r="H52" s="115"/>
-      <c r="I52" s="116"/>
+      <c r="H52" s="84"/>
+      <c r="I52" s="85"/>
       <c r="J52" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="53" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="90"/>
-      <c r="E53" s="93"/>
-      <c r="F53" s="113"/>
+      <c r="D53" s="77"/>
+      <c r="E53" s="79"/>
+      <c r="F53" s="81"/>
       <c r="G53" s="59">
         <v>0.38</v>
       </c>
-      <c r="H53" s="117"/>
-      <c r="I53" s="118"/>
+      <c r="H53" s="86"/>
+      <c r="I53" s="87"/>
       <c r="J53" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="54" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="111"/>
+      <c r="D54" s="78"/>
       <c r="E54" s="45"/>
       <c r="F54" s="45"/>
       <c r="G54" s="46"/>
@@ -8094,53 +8146,53 @@
       <c r="J54" s="47"/>
     </row>
     <row r="55" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D55" s="90"/>
-      <c r="E55" s="92" t="s">
+      <c r="D55" s="77"/>
+      <c r="E55" s="76" t="s">
         <v>419</v>
       </c>
-      <c r="F55" s="112" t="s">
+      <c r="F55" s="80" t="s">
         <v>420</v>
       </c>
       <c r="G55" s="60">
         <v>0.25</v>
       </c>
-      <c r="H55" s="80" t="s">
+      <c r="H55" s="82" t="s">
         <v>403</v>
       </c>
-      <c r="I55" s="81"/>
+      <c r="I55" s="90"/>
       <c r="J55" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="56" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D56" s="90"/>
-      <c r="E56" s="90"/>
-      <c r="F56" s="111"/>
+      <c r="D56" s="77"/>
+      <c r="E56" s="77"/>
+      <c r="F56" s="78"/>
       <c r="G56" s="42">
         <v>0.35</v>
       </c>
-      <c r="H56" s="121"/>
-      <c r="I56" s="122"/>
+      <c r="H56" s="93"/>
+      <c r="I56" s="94"/>
       <c r="J56" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="57" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D57" s="90"/>
-      <c r="E57" s="90"/>
-      <c r="F57" s="113"/>
+      <c r="D57" s="77"/>
+      <c r="E57" s="77"/>
+      <c r="F57" s="81"/>
       <c r="G57" s="59">
         <v>0.38</v>
       </c>
-      <c r="H57" s="82"/>
-      <c r="I57" s="83"/>
+      <c r="H57" s="91"/>
+      <c r="I57" s="92"/>
       <c r="J57" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="58" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="90"/>
-      <c r="E58" s="111"/>
+      <c r="D58" s="77"/>
+      <c r="E58" s="78"/>
       <c r="F58" s="45"/>
       <c r="G58" s="46"/>
       <c r="H58" s="46"/>
@@ -8148,50 +8200,50 @@
       <c r="J58" s="47"/>
     </row>
     <row r="59" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D59" s="90"/>
-      <c r="E59" s="90"/>
-      <c r="F59" s="112" t="s">
+      <c r="D59" s="77"/>
+      <c r="E59" s="77"/>
+      <c r="F59" s="80" t="s">
         <v>426</v>
       </c>
       <c r="G59" s="60">
         <v>0.25</v>
       </c>
-      <c r="H59" s="80" t="s">
+      <c r="H59" s="82" t="s">
         <v>403</v>
       </c>
-      <c r="I59" s="81"/>
+      <c r="I59" s="90"/>
       <c r="J59" s="41">
         <v>14</v>
       </c>
     </row>
     <row r="60" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D60" s="90"/>
-      <c r="E60" s="90"/>
-      <c r="F60" s="111"/>
+      <c r="D60" s="77"/>
+      <c r="E60" s="77"/>
+      <c r="F60" s="78"/>
       <c r="G60" s="42">
         <v>0.35</v>
       </c>
-      <c r="H60" s="121"/>
-      <c r="I60" s="122"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="94"/>
       <c r="J60" s="43">
         <v>14</v>
       </c>
     </row>
     <row r="61" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D61" s="90"/>
-      <c r="E61" s="93"/>
-      <c r="F61" s="113"/>
+      <c r="D61" s="77"/>
+      <c r="E61" s="79"/>
+      <c r="F61" s="81"/>
       <c r="G61" s="59">
         <v>0.38</v>
       </c>
-      <c r="H61" s="82"/>
-      <c r="I61" s="83"/>
+      <c r="H61" s="91"/>
+      <c r="I61" s="92"/>
       <c r="J61" s="44">
         <v>14</v>
       </c>
     </row>
     <row r="62" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D62" s="90"/>
+      <c r="D62" s="77"/>
       <c r="E62" s="52"/>
       <c r="F62" s="45"/>
       <c r="G62" s="46"/>
@@ -8200,33 +8252,33 @@
       <c r="J62" s="47"/>
     </row>
     <row r="63" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D63" s="90"/>
-      <c r="E63" s="112" t="s">
+      <c r="D63" s="77"/>
+      <c r="E63" s="80" t="s">
         <v>422</v>
       </c>
-      <c r="F63" s="119" t="s">
+      <c r="F63" s="88" t="s">
         <v>423</v>
       </c>
       <c r="G63" s="60">
         <v>0.25</v>
       </c>
-      <c r="H63" s="80" t="s">
+      <c r="H63" s="82" t="s">
         <v>424</v>
       </c>
-      <c r="I63" s="81"/>
+      <c r="I63" s="90"/>
       <c r="J63" s="41">
         <v>1</v>
       </c>
     </row>
     <row r="64" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D64" s="93"/>
-      <c r="E64" s="113"/>
-      <c r="F64" s="120"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="81"/>
+      <c r="F64" s="89"/>
       <c r="G64" s="59">
         <v>0.38</v>
       </c>
-      <c r="H64" s="82"/>
-      <c r="I64" s="83"/>
+      <c r="H64" s="91"/>
+      <c r="I64" s="92"/>
       <c r="J64" s="44">
         <v>1</v>
       </c>
@@ -8248,6 +8300,47 @@
     </row>
   </sheetData>
   <mergeCells count="55">
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D11:D26"/>
+    <mergeCell ref="E11:E19"/>
+    <mergeCell ref="F13:F17"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="F25:F26"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="D28:D45"/>
+    <mergeCell ref="E28:E34"/>
+    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="H28:I30"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="H32:I34"/>
+    <mergeCell ref="E36:E42"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="H36:I38"/>
+    <mergeCell ref="F40:F42"/>
+    <mergeCell ref="H40:I42"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="F44:F45"/>
+    <mergeCell ref="H44:I45"/>
     <mergeCell ref="D47:D64"/>
     <mergeCell ref="E47:E53"/>
     <mergeCell ref="F47:F49"/>
@@ -8262,47 +8355,6 @@
     <mergeCell ref="H55:I57"/>
     <mergeCell ref="F59:F61"/>
     <mergeCell ref="H59:I61"/>
-    <mergeCell ref="D28:D45"/>
-    <mergeCell ref="E28:E34"/>
-    <mergeCell ref="F28:F30"/>
-    <mergeCell ref="H28:I30"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="H32:I34"/>
-    <mergeCell ref="E36:E42"/>
-    <mergeCell ref="F36:F38"/>
-    <mergeCell ref="H36:I38"/>
-    <mergeCell ref="F40:F42"/>
-    <mergeCell ref="H40:I42"/>
-    <mergeCell ref="E44:E45"/>
-    <mergeCell ref="F44:F45"/>
-    <mergeCell ref="H44:I45"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F23"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="F25:F26"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D11:D26"/>
-    <mergeCell ref="E11:E19"/>
-    <mergeCell ref="F13:F17"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -12957,4 +13009,1256 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA648938-26BA-459E-AB8B-405148DB51EC}">
+  <dimension ref="C2:N91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:14" ht="40.799999999999997" x14ac:dyDescent="0.75">
+      <c r="C2" s="123" t="s">
+        <v>507</v>
+      </c>
+      <c r="I2" s="123" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="3:14" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="C5" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>509</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="N5" s="54" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.99006072525323596</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.99993909635221401</v>
+      </c>
+    </row>
+    <row r="7" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C7">
+        <v>2.2893819412499998</v>
+      </c>
+      <c r="D7">
+        <v>0.97844997684405499</v>
+      </c>
+      <c r="I7">
+        <v>2.6263631807496099</v>
+      </c>
+      <c r="J7">
+        <v>0.98822090259267004</v>
+      </c>
+    </row>
+    <row r="8" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C8">
+        <v>2.4405248522499998</v>
+      </c>
+      <c r="D8">
+        <v>0.96683920795202904</v>
+      </c>
+      <c r="I8">
+        <v>2.9013386207584801</v>
+      </c>
+      <c r="J8">
+        <v>0.97650268862816803</v>
+      </c>
+    </row>
+    <row r="9" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C9">
+        <v>2.540740182</v>
+      </c>
+      <c r="D9">
+        <v>0.95522846233032999</v>
+      </c>
+      <c r="I9">
+        <v>3.0699245291638899</v>
+      </c>
+      <c r="J9">
+        <v>0.96478447634211295</v>
+      </c>
+    </row>
+    <row r="10" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C10">
+        <v>2.6087488890000001</v>
+      </c>
+      <c r="D10">
+        <v>0.94361769624540903</v>
+      </c>
+      <c r="I10">
+        <v>3.1839835469061901</v>
+      </c>
+      <c r="J10">
+        <v>0.95306626574641995</v>
+      </c>
+    </row>
+    <row r="11" spans="3:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>2.6731142194999999</v>
+      </c>
+      <c r="D11">
+        <v>0.93200693157891701</v>
+      </c>
+      <c r="I11">
+        <v>3.29137679241517</v>
+      </c>
+      <c r="J11">
+        <v>0.94134805685311096</v>
+      </c>
+      <c r="M11" s="124" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="12" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C12">
+        <v>2.7321392680000001</v>
+      </c>
+      <c r="D12">
+        <v>0.92039619021258301</v>
+      </c>
+      <c r="I12">
+        <v>3.3804114517631398</v>
+      </c>
+      <c r="J12">
+        <v>0.92962987154591503</v>
+      </c>
+      <c r="M12" s="125" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="13" spans="3:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C13">
+        <v>2.7844395662500001</v>
+      </c>
+      <c r="D13">
+        <v>0.90878542841315602</v>
+      </c>
+      <c r="I13">
+        <v>3.4553766589044099</v>
+      </c>
+      <c r="J13">
+        <v>0.91791166609390695</v>
+      </c>
+      <c r="M13" s="125" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="14" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C14">
+        <v>2.8299418854999998</v>
+      </c>
+      <c r="D14">
+        <v>0.89717466806256496</v>
+      </c>
+      <c r="I14">
+        <v>3.5219753734752701</v>
+      </c>
+      <c r="J14">
+        <v>0.90619346238105003</v>
+      </c>
+    </row>
+    <row r="15" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C15">
+        <v>2.8695722890000002</v>
+      </c>
+      <c r="D15">
+        <v>0.88556393104282005</v>
+      </c>
+      <c r="I15">
+        <v>3.5784521882900799</v>
+      </c>
+      <c r="J15">
+        <v>0.89447526041983305</v>
+      </c>
+    </row>
+    <row r="16" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C16">
+        <v>2.9046735309999998</v>
+      </c>
+      <c r="D16">
+        <v>0.87395317362097902</v>
+      </c>
+      <c r="I16">
+        <v>3.62654105256154</v>
+      </c>
+      <c r="J16">
+        <v>0.88275706022286904</v>
+      </c>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>2.9351762162499999</v>
+      </c>
+      <c r="D17">
+        <v>0.86234243955093204</v>
+      </c>
+      <c r="I17">
+        <v>3.67366940785096</v>
+      </c>
+      <c r="J17">
+        <v>0.87103888367446003</v>
+      </c>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>2.96345672625</v>
+      </c>
+      <c r="D18">
+        <v>0.85073168509995001</v>
+      </c>
+      <c r="I18">
+        <v>3.7225151534708401</v>
+      </c>
+      <c r="J18">
+        <v>0.85932068704431197</v>
+      </c>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>2.9907246052500001</v>
+      </c>
+      <c r="D19">
+        <v>0.83912093215044004</v>
+      </c>
+      <c r="I19">
+        <v>3.7656705573297899</v>
+      </c>
+      <c r="J19">
+        <v>0.84760249221698103</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>3.01775316225</v>
+      </c>
+      <c r="D20">
+        <v>0.82751020258490704</v>
+      </c>
+      <c r="I20">
+        <v>3.8109133213572801</v>
+      </c>
+      <c r="J20">
+        <v>0.83588429920556995</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>3.04475775475</v>
+      </c>
+      <c r="D21">
+        <v>0.81589945267094599</v>
+      </c>
+      <c r="I21">
+        <v>3.86267101219783</v>
+      </c>
+      <c r="J21">
+        <v>0.82416610802331203</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>3.07366259425</v>
+      </c>
+      <c r="D22">
+        <v>0.80428870429127097</v>
+      </c>
+      <c r="I22">
+        <v>3.9123574479929002</v>
+      </c>
+      <c r="J22">
+        <v>0.81244794055512104</v>
+      </c>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>3.1029355624999999</v>
+      </c>
+      <c r="D23">
+        <v>0.792677979328692</v>
+      </c>
+      <c r="I23">
+        <v>3.9572268982035901</v>
+      </c>
+      <c r="J23">
+        <v>0.80072975307137695</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>3.13272962975</v>
+      </c>
+      <c r="D24">
+        <v>0.78106723405114498</v>
+      </c>
+      <c r="I24">
+        <v>4.0001335792858699</v>
+      </c>
+      <c r="J24">
+        <v>0.78901156745725898</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>3.1647982727500001</v>
+      </c>
+      <c r="D25">
+        <v>0.76945651221331501</v>
+      </c>
+      <c r="I25">
+        <v>4.0402613220226202</v>
+      </c>
+      <c r="J25">
+        <v>0.77729338372652501</v>
+      </c>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>3.20032342375</v>
+      </c>
+      <c r="D26">
+        <v>0.75784577008336795</v>
+      </c>
+      <c r="I26">
+        <v>4.0775959252605896</v>
+      </c>
+      <c r="J26">
+        <v>0.76557520189306705</v>
+      </c>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>3.23448136825</v>
+      </c>
+      <c r="D27">
+        <v>0.74623502954455401</v>
+      </c>
+      <c r="I27">
+        <v>4.1186627272122402</v>
+      </c>
+      <c r="J27">
+        <v>0.75385704384245</v>
+      </c>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>3.2687084357499998</v>
+      </c>
+      <c r="D28">
+        <v>0.73462431248022297</v>
+      </c>
+      <c r="I28">
+        <v>4.1665681057884196</v>
+      </c>
+      <c r="J28">
+        <v>0.74213886584576505</v>
+      </c>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>3.30485967675</v>
+      </c>
+      <c r="D29">
+        <v>0.72301357515889897</v>
+      </c>
+      <c r="I29">
+        <v>4.21700471190952</v>
+      </c>
+      <c r="J29">
+        <v>0.73042068978885999</v>
+      </c>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>3.3417323219999999</v>
+      </c>
+      <c r="D30">
+        <v>0.71140286133580699</v>
+      </c>
+      <c r="I30">
+        <v>4.2659249427811101</v>
+      </c>
+      <c r="J30">
+        <v>0.71870251568618604</v>
+      </c>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>3.37746461375</v>
+      </c>
+      <c r="D31">
+        <v>0.69979212727972095</v>
+      </c>
+      <c r="I31">
+        <v>4.3107375371479302</v>
+      </c>
+      <c r="J31">
+        <v>0.70698434355233597</v>
+      </c>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>3.4126825945000001</v>
+      </c>
+      <c r="D32">
+        <v>0.68818139487445495</v>
+      </c>
+      <c r="I32">
+        <v>4.3544153155910399</v>
+      </c>
+      <c r="J32">
+        <v>0.69526619527356903</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>3.4440332282499999</v>
+      </c>
+      <c r="D33">
+        <v>0.676570686003934</v>
+      </c>
+      <c r="I33">
+        <v>4.3982775579951197</v>
+      </c>
+      <c r="J33">
+        <v>0.68354802712173102</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>3.4709187747499999</v>
+      </c>
+      <c r="D34">
+        <v>0.66495995693731402</v>
+      </c>
+      <c r="I34">
+        <v>4.4470615176314103</v>
+      </c>
+      <c r="J34">
+        <v>0.67182986098338004</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>3.4965185557499998</v>
+      </c>
+      <c r="D35">
+        <v>0.65334922955876595</v>
+      </c>
+      <c r="I35">
+        <v>4.4997794648480802</v>
+      </c>
+      <c r="J35">
+        <v>0.66011169687370497</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>3.5238947237499998</v>
+      </c>
+      <c r="D36">
+        <v>0.64173852575257795</v>
+      </c>
+      <c r="I36">
+        <v>4.5475176815258402</v>
+      </c>
+      <c r="J36">
+        <v>0.64839353480804596</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>3.5554500382500001</v>
+      </c>
+      <c r="D37">
+        <v>0.63012780178829997</v>
+      </c>
+      <c r="I37">
+        <v>4.5921074267021504</v>
+      </c>
+      <c r="J37">
+        <v>0.63667539667339901</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>3.5906158659999998</v>
+      </c>
+      <c r="D38">
+        <v>0.61851710142209104</v>
+      </c>
+      <c r="I38">
+        <v>4.6404006799733901</v>
+      </c>
+      <c r="J38">
+        <v>0.62495723874241305</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C39">
+        <v>3.6249534252500002</v>
+      </c>
+      <c r="D39">
+        <v>0.60690638092377003</v>
+      </c>
+      <c r="I39">
+        <v>4.6915620691949398</v>
+      </c>
+      <c r="J39">
+        <v>0.61323908290240503</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C40">
+        <v>3.6567667099999999</v>
+      </c>
+      <c r="D40">
+        <v>0.59529566217814101</v>
+      </c>
+      <c r="I40">
+        <v>4.7428077134619704</v>
+      </c>
+      <c r="J40">
+        <v>0.60152092916934696</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C41">
+        <v>3.6881186942499999</v>
+      </c>
+      <c r="D41">
+        <v>0.58368496707012596</v>
+      </c>
+      <c r="I41">
+        <v>4.7928863825682004</v>
+      </c>
+      <c r="J41">
+        <v>0.58980277755937505</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C42">
+        <v>3.7187081040000001</v>
+      </c>
+      <c r="D42">
+        <v>0.57207425186996497</v>
+      </c>
+      <c r="I42">
+        <v>4.83963513883345</v>
+      </c>
+      <c r="J42">
+        <v>0.57808464996026898</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C43">
+        <v>3.7478520637499999</v>
+      </c>
+      <c r="D43">
+        <v>0.56046353846285601</v>
+      </c>
+      <c r="I43">
+        <v>4.87822446174318</v>
+      </c>
+      <c r="J43">
+        <v>0.56636650264553701</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C44">
+        <v>3.7777530582500001</v>
+      </c>
+      <c r="D44">
+        <v>0.54885284873411999</v>
+      </c>
+      <c r="I44">
+        <v>4.9153031465956998</v>
+      </c>
+      <c r="J44">
+        <v>0.55464835750329899</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C45">
+        <v>3.8073059704999999</v>
+      </c>
+      <c r="D45">
+        <v>0.53724213895443795</v>
+      </c>
+      <c r="I45">
+        <v>4.9571803291195398</v>
+      </c>
+      <c r="J45">
+        <v>0.54293021455036505</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C46">
+        <v>3.8352902327499998</v>
+      </c>
+      <c r="D46">
+        <v>0.52563145288100499</v>
+      </c>
+      <c r="I46">
+        <v>4.9983165225105299</v>
+      </c>
+      <c r="J46">
+        <v>0.53121207380371804</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C47">
+        <v>3.8628227965000002</v>
+      </c>
+      <c r="D47">
+        <v>0.51402074678479603</v>
+      </c>
+      <c r="I47">
+        <v>5.0364951681082299</v>
+      </c>
+      <c r="J47">
+        <v>0.51949395715197799</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C48">
+        <v>3.8901339202499998</v>
+      </c>
+      <c r="D48">
+        <v>0.50241004255170696</v>
+      </c>
+      <c r="I48">
+        <v>5.07151040807274</v>
+      </c>
+      <c r="J48">
+        <v>0.50777582086955997</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C49">
+        <v>3.9151950907500002</v>
+      </c>
+      <c r="D49">
+        <v>0.49079936206776298</v>
+      </c>
+      <c r="I49">
+        <v>5.1046893892215603</v>
+      </c>
+      <c r="J49">
+        <v>0.49605768684544599</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C50">
+        <v>3.9371720015</v>
+      </c>
+      <c r="D50">
+        <v>0.47918866160440499</v>
+      </c>
+      <c r="I50">
+        <v>5.1387403530716398</v>
+      </c>
+      <c r="J50">
+        <v>0.484339555097338</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C51">
+        <v>3.95536121025</v>
+      </c>
+      <c r="D51">
+        <v>0.467577963047967</v>
+      </c>
+      <c r="I51">
+        <v>5.1760668046129998</v>
+      </c>
+      <c r="J51">
+        <v>0.47262142564312398</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C52">
+        <v>3.9687882507499999</v>
+      </c>
+      <c r="D52">
+        <v>0.45596728828491701</v>
+      </c>
+      <c r="I52">
+        <v>5.20902842603682</v>
+      </c>
+      <c r="J52">
+        <v>0.46090332037231801</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C53">
+        <v>3.9813272044999999</v>
+      </c>
+      <c r="D53">
+        <v>0.44435659358718199</v>
+      </c>
+      <c r="I53">
+        <v>5.2354429935684204</v>
+      </c>
+      <c r="J53">
+        <v>0.44918519556030301</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C54">
+        <v>3.9956767575000001</v>
+      </c>
+      <c r="D54">
+        <v>0.43274592271310802</v>
+      </c>
+      <c r="I54">
+        <v>5.2549592202262199</v>
+      </c>
+      <c r="J54">
+        <v>0.43746707309698102</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C55">
+        <v>4.0089201604999998</v>
+      </c>
+      <c r="D55">
+        <v>0.421135231934952</v>
+      </c>
+      <c r="I55">
+        <v>5.26941828498558</v>
+      </c>
+      <c r="J55">
+        <v>0.42574895300100801</v>
+      </c>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C56">
+        <v>4.0208868669999998</v>
+      </c>
+      <c r="D56">
+        <v>0.40952454313981701</v>
+      </c>
+      <c r="I56">
+        <v>5.2803063413173703</v>
+      </c>
+      <c r="J56">
+        <v>0.41403083529123302</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C57">
+        <v>4.0302657397499999</v>
+      </c>
+      <c r="D57">
+        <v>0.397913878214953</v>
+      </c>
+      <c r="I57">
+        <v>5.2905574136172104</v>
+      </c>
+      <c r="J57">
+        <v>0.40231274185812899</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C58">
+        <v>4.0386687349999999</v>
+      </c>
+      <c r="D58">
+        <v>0.38630319343313402</v>
+      </c>
+      <c r="I58">
+        <v>5.3051187964071902</v>
+      </c>
+      <c r="J58">
+        <v>0.39059462897811298</v>
+      </c>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C59">
+        <v>4.0468993482500002</v>
+      </c>
+      <c r="D59">
+        <v>0.37469251068194898</v>
+      </c>
+      <c r="I59">
+        <v>5.3184326595697504</v>
+      </c>
+      <c r="J59">
+        <v>0.378876518542068</v>
+      </c>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C60">
+        <v>4.0558327214999998</v>
+      </c>
+      <c r="D60">
+        <v>0.36308185184914399</v>
+      </c>
+      <c r="I60">
+        <v>5.3283700578842303</v>
+      </c>
+      <c r="J60">
+        <v>0.36715841056966603</v>
+      </c>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C61">
+        <v>4.0647901329999998</v>
+      </c>
+      <c r="D61">
+        <v>0.35147117320802401</v>
+      </c>
+      <c r="I61">
+        <v>5.3361641437125797</v>
+      </c>
+      <c r="J61">
+        <v>0.355440305080791</v>
+      </c>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C62">
+        <v>4.0733980660000002</v>
+      </c>
+      <c r="D62">
+        <v>0.33986051851821802</v>
+      </c>
+      <c r="I62">
+        <v>5.3424651066755402</v>
+      </c>
+      <c r="J62">
+        <v>0.34372222396693097</v>
+      </c>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C63">
+        <v>4.0796562200000004</v>
+      </c>
+      <c r="D63">
+        <v>0.32824984405340002</v>
+      </c>
+      <c r="I63">
+        <v>5.3429511982701303</v>
+      </c>
+      <c r="J63">
+        <v>0.33200412350561098</v>
+      </c>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C64">
+        <v>4.08297912975</v>
+      </c>
+      <c r="D64">
+        <v>0.316639171702017</v>
+      </c>
+      <c r="I64">
+        <v>5.3391329731647801</v>
+      </c>
+      <c r="J64">
+        <v>0.32028602558876501</v>
+      </c>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C65">
+        <v>4.0857462890000003</v>
+      </c>
+      <c r="D65">
+        <v>0.30502852335268499</v>
+      </c>
+      <c r="I65">
+        <v>5.3384903242404098</v>
+      </c>
+      <c r="J65">
+        <v>0.30856793023715101</v>
+      </c>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C66">
+        <v>4.0904372320000002</v>
+      </c>
+      <c r="D66">
+        <v>0.29341785527964798</v>
+      </c>
+      <c r="I66">
+        <v>5.3365201716566899</v>
+      </c>
+      <c r="J66">
+        <v>0.29684983747175397</v>
+      </c>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C67">
+        <v>4.09587117425</v>
+      </c>
+      <c r="D67">
+        <v>0.28180718937189903</v>
+      </c>
+      <c r="I67">
+        <v>5.3325627828786901</v>
+      </c>
+      <c r="J67">
+        <v>0.28513176918515698</v>
+      </c>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C68">
+        <v>4.0989064557499999</v>
+      </c>
+      <c r="D68">
+        <v>0.270196547518601</v>
+      </c>
+      <c r="I68">
+        <v>5.3342969543135998</v>
+      </c>
+      <c r="J68">
+        <v>0.273413681656066</v>
+      </c>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C69">
+        <v>4.09813326</v>
+      </c>
+      <c r="D69">
+        <v>0.25858588599459498</v>
+      </c>
+      <c r="I69">
+        <v>5.3396583843424299</v>
+      </c>
+      <c r="J69">
+        <v>0.26169559677753701</v>
+      </c>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C70">
+        <v>4.0932968437500001</v>
+      </c>
+      <c r="D70">
+        <v>0.246975248560933</v>
+      </c>
+      <c r="I70">
+        <v>5.3385672317587103</v>
+      </c>
+      <c r="J70">
+        <v>0.249977514571492</v>
+      </c>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C71">
+        <v>4.0838281217499999</v>
+      </c>
+      <c r="D71">
+        <v>0.23536459149286801</v>
+      </c>
+      <c r="I71">
+        <v>5.3255683557329796</v>
+      </c>
+      <c r="J71">
+        <v>0.238259435060096</v>
+      </c>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C72">
+        <v>4.0703856137500001</v>
+      </c>
+      <c r="D72">
+        <v>0.22375393668034399</v>
+      </c>
+      <c r="I72">
+        <v>5.3067820057662498</v>
+      </c>
+      <c r="J72">
+        <v>0.22654138013710201</v>
+      </c>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C73">
+        <v>4.0521489565</v>
+      </c>
+      <c r="D73">
+        <v>0.21214330601349299</v>
+      </c>
+      <c r="I73">
+        <v>5.2834213333333304</v>
+      </c>
+      <c r="J73">
+        <v>0.21482330608247799</v>
+      </c>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C74">
+        <v>4.0292916595000001</v>
+      </c>
+      <c r="D74">
+        <v>0.20053265576820301</v>
+      </c>
+      <c r="I74">
+        <v>5.2489792636948298</v>
+      </c>
+      <c r="J74">
+        <v>0.203105234790487</v>
+      </c>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C75">
+        <v>4.0023536254999996</v>
+      </c>
+      <c r="D75">
+        <v>0.18892200783502699</v>
+      </c>
+      <c r="I75">
+        <v>5.2049873455311602</v>
+      </c>
+      <c r="J75">
+        <v>0.191387166284294</v>
+      </c>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C76">
+        <v>3.9693018000000002</v>
+      </c>
+      <c r="D76">
+        <v>0.17731138410471001</v>
+      </c>
+      <c r="I76">
+        <v>5.1555231896207596</v>
+      </c>
+      <c r="J76">
+        <v>0.17966910058732999</v>
+      </c>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C77">
+        <v>3.9296699479999999</v>
+      </c>
+      <c r="D77">
+        <v>0.16570074085380099</v>
+      </c>
+      <c r="I77">
+        <v>5.0971001936127802</v>
+      </c>
+      <c r="J77">
+        <v>0.16795105959460299</v>
+      </c>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C78">
+        <v>3.8853915964999999</v>
+      </c>
+      <c r="D78">
+        <v>0.154090121844947</v>
+      </c>
+      <c r="I78">
+        <v>5.0281025832778896</v>
+      </c>
+      <c r="J78">
+        <v>0.15623299958743</v>
+      </c>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C79">
+        <v>3.8372255432500002</v>
+      </c>
+      <c r="D79">
+        <v>0.14247948335515001</v>
+      </c>
+      <c r="I79">
+        <v>4.95309939277002</v>
+      </c>
+      <c r="J79">
+        <v>0.14451494246136701</v>
+      </c>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C80">
+        <v>3.7819877745000001</v>
+      </c>
+      <c r="D80">
+        <v>0.13086884727603099</v>
+      </c>
+      <c r="I80">
+        <v>4.8724739332446196</v>
+      </c>
+      <c r="J80">
+        <v>0.13279688824091401</v>
+      </c>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C81">
+        <v>3.7208441142500002</v>
+      </c>
+      <c r="D81">
+        <v>0.11925823549942</v>
+      </c>
+      <c r="I81">
+        <v>4.7826662468396499</v>
+      </c>
+      <c r="J81">
+        <v>0.121078836950858</v>
+      </c>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C82">
+        <v>3.6488373527500002</v>
+      </c>
+      <c r="D82">
+        <v>0.107647604303031</v>
+      </c>
+      <c r="I82">
+        <v>4.6831459068529604</v>
+      </c>
+      <c r="J82">
+        <v>0.109360810487555</v>
+      </c>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C83">
+        <v>3.5700807229999998</v>
+      </c>
+      <c r="D83">
+        <v>9.60369974505971E-2</v>
+      </c>
+      <c r="I83">
+        <v>4.5764722920825003</v>
+      </c>
+      <c r="J83">
+        <v>9.7642765133769294E-2</v>
+      </c>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C84">
+        <v>3.4850482540000001</v>
+      </c>
+      <c r="D84">
+        <v>8.4426371220325397E-2</v>
+      </c>
+      <c r="I84">
+        <v>4.4718568374362402</v>
+      </c>
+      <c r="J84">
+        <v>8.5924722786440894E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C85">
+        <v>3.3966062639999999</v>
+      </c>
+      <c r="D85">
+        <v>7.2815747504980294E-2</v>
+      </c>
+      <c r="I85">
+        <v>4.3626942816589001</v>
+      </c>
+      <c r="J85">
+        <v>7.4206683471509299E-2</v>
+      </c>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C86">
+        <v>3.3187059617500001</v>
+      </c>
+      <c r="D86">
+        <v>6.1205148197552101E-2</v>
+      </c>
+      <c r="I86">
+        <v>4.23425836837436</v>
+      </c>
+      <c r="J86">
+        <v>6.24886472152094E-2</v>
+      </c>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C87">
+        <v>3.2330801015000001</v>
+      </c>
+      <c r="D87">
+        <v>4.9594529577004103E-2</v>
+      </c>
+      <c r="I87">
+        <v>4.01740089820359</v>
+      </c>
+      <c r="J87">
+        <v>5.0770635915347903E-2</v>
+      </c>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C88">
+        <v>3.0927073025</v>
+      </c>
+      <c r="D88">
+        <v>3.79839135368309E-2</v>
+      </c>
+      <c r="I88">
+        <v>3.64556676890663</v>
+      </c>
+      <c r="J88">
+        <v>3.9052605856240701E-2</v>
+      </c>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C89">
+        <v>2.01193701025</v>
+      </c>
+      <c r="D89">
+        <v>2.63733219707608E-2</v>
+      </c>
+      <c r="I89">
+        <v>3.1462934391217598</v>
+      </c>
+      <c r="J89">
+        <v>2.7334578936318101E-2</v>
+      </c>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>1.47627111585504E-2</v>
+      </c>
+      <c r="I90">
+        <v>2.2304782501663301</v>
+      </c>
+      <c r="J90">
+        <v>1.56165551830594E-2</v>
+      </c>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="I91">
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>3.8985346242641199E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>